<commit_message>
Added worked hours to Project Schedule
</commit_message>
<xml_diff>
--- a/Project Schedule.xlsx
+++ b/Project Schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="842" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="842" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Some Hints and Explanations" sheetId="3" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="168">
   <si>
     <t>Typ</t>
   </si>
@@ -525,6 +525,39 @@
   <si>
     <t>Set up Project Mgmt Tools</t>
   </si>
+  <si>
+    <t>Research and set up Project Mgmt Tools</t>
+  </si>
+  <si>
+    <t>13.4.15 - 15.04.15</t>
+  </si>
+  <si>
+    <t>Research application ideas</t>
+  </si>
+  <si>
+    <t>18.4.</t>
+  </si>
+  <si>
+    <t>20.4.</t>
+  </si>
+  <si>
+    <t>Project Schedule Template</t>
+  </si>
+  <si>
+    <t>Research Data Sets</t>
+  </si>
+  <si>
+    <t>20.4., 21.04.</t>
+  </si>
+  <si>
+    <t>Team Meeting 2: Tutorials &amp; Poster Ideas</t>
+  </si>
+  <si>
+    <t>23.4.</t>
+  </si>
+  <si>
+    <t>Team Meeting 1: Application Idea &amp; Schedule</t>
+  </si>
 </sst>
 </file>
 
@@ -935,7 +968,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -944,7 +980,7 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="15" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="12" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -953,13 +989,10 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="15" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -969,72 +1002,7 @@
     <cellStyle name="Heading 4" xfId="3" builtinId="19"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <b/>
@@ -1211,25 +1179,6 @@
       <font>
         <b/>
         <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
       </font>
       <fill>
         <patternFill>
@@ -1251,8 +1200,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="28"/>
-      <tableStyleElement type="headerRow" dxfId="27"/>
+      <tableStyleElement type="wholeTable" dxfId="19"/>
+      <tableStyleElement type="headerRow" dxfId="18"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -4697,37 +4646,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A36:B321">
-    <cfRule type="expression" dxfId="13" priority="114">
+    <cfRule type="expression" dxfId="6" priority="114">
       <formula>(#REF!="M")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7:XFD35 A36:XFD320">
-    <cfRule type="expression" dxfId="12" priority="116">
+    <cfRule type="expression" dxfId="5" priority="116">
       <formula>(#REF!="M")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:B35">
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>(MID($A35,2,1)="M")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:L5 A7:L35">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>(MID($A3,2,1)="M")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B5 A7:B35">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>(MID($A3,2,1)="M")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:L6">
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>(MID($A6,2,1)="M")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B6">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>(MID($A6,2,1)="M")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9187,17 +9136,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A15:B302">
-    <cfRule type="expression" dxfId="24" priority="79">
+    <cfRule type="expression" dxfId="17" priority="79">
       <formula>(MID($A15,2,1)="M")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:XFD300">
-    <cfRule type="expression" dxfId="23" priority="83">
+    <cfRule type="expression" dxfId="16" priority="83">
       <formula>(MID($A3,2,1)="M")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B300">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>(MID($A3,2,1)="M")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9209,7 +9158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CZ430"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="128" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="128" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -9256,385 +9205,385 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:104" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="57"/>
-      <c r="AD1" s="57"/>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="57"/>
-      <c r="AG1" s="57"/>
-      <c r="AH1" s="57"/>
-      <c r="AI1" s="57"/>
-      <c r="AJ1" s="57"/>
-      <c r="AK1" s="57"/>
-      <c r="AL1" s="57"/>
-      <c r="AM1" s="57"/>
-      <c r="AN1" s="57"/>
-      <c r="AO1" s="57"/>
-      <c r="AP1" s="57"/>
-      <c r="AQ1" s="57"/>
-      <c r="AR1" s="57"/>
-      <c r="AS1" s="57"/>
-      <c r="AT1" s="57"/>
-      <c r="AU1" s="57"/>
-      <c r="AV1" s="57"/>
-      <c r="AW1" s="57"/>
-      <c r="AX1" s="57"/>
-      <c r="AY1" s="57"/>
-      <c r="AZ1" s="57"/>
-      <c r="BA1" s="57"/>
-      <c r="BB1" s="57"/>
-      <c r="BC1" s="57"/>
-      <c r="BD1" s="57"/>
-      <c r="BE1" s="57"/>
-      <c r="BF1" s="57"/>
-      <c r="BG1" s="57"/>
-      <c r="BH1" s="57"/>
-      <c r="BI1" s="57"/>
-      <c r="BJ1" s="57"/>
-      <c r="BK1" s="57"/>
-      <c r="BL1" s="57"/>
-      <c r="BM1" s="57"/>
-      <c r="BN1" s="57"/>
-      <c r="BO1" s="57"/>
-      <c r="BP1" s="57"/>
-      <c r="BQ1" s="57"/>
-      <c r="BR1" s="57"/>
-      <c r="BS1" s="57"/>
-      <c r="BT1" s="57"/>
-      <c r="BU1" s="57"/>
-      <c r="BV1" s="57"/>
-      <c r="BW1" s="57"/>
-      <c r="BX1" s="57"/>
-      <c r="BY1" s="57"/>
-      <c r="BZ1" s="57"/>
-      <c r="CA1" s="57"/>
-      <c r="CB1" s="57"/>
-      <c r="CC1" s="57"/>
-      <c r="CD1" s="57"/>
-      <c r="CE1" s="57"/>
-      <c r="CF1" s="57"/>
-      <c r="CG1" s="57"/>
-      <c r="CH1" s="57"/>
-      <c r="CI1" s="57"/>
-      <c r="CJ1" s="57"/>
-      <c r="CK1" s="57"/>
-      <c r="CL1" s="57"/>
-      <c r="CM1" s="57"/>
-      <c r="CN1" s="57"/>
-      <c r="CO1" s="57"/>
-      <c r="CP1" s="57"/>
-      <c r="CQ1" s="57"/>
-      <c r="CR1" s="57"/>
-      <c r="CS1" s="57"/>
-      <c r="CT1" s="57"/>
-      <c r="CU1" s="57"/>
-      <c r="CV1" s="57"/>
-      <c r="CW1" s="57"/>
-      <c r="CX1" s="57"/>
-      <c r="CY1" s="57"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AN1" s="51"/>
+      <c r="AO1" s="51"/>
+      <c r="AP1" s="51"/>
+      <c r="AQ1" s="51"/>
+      <c r="AR1" s="51"/>
+      <c r="AS1" s="51"/>
+      <c r="AT1" s="51"/>
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="51"/>
+      <c r="AW1" s="51"/>
+      <c r="AX1" s="51"/>
+      <c r="AY1" s="51"/>
+      <c r="AZ1" s="51"/>
+      <c r="BA1" s="51"/>
+      <c r="BB1" s="51"/>
+      <c r="BC1" s="51"/>
+      <c r="BD1" s="51"/>
+      <c r="BE1" s="51"/>
+      <c r="BF1" s="51"/>
+      <c r="BG1" s="51"/>
+      <c r="BH1" s="51"/>
+      <c r="BI1" s="51"/>
+      <c r="BJ1" s="51"/>
+      <c r="BK1" s="51"/>
+      <c r="BL1" s="51"/>
+      <c r="BM1" s="51"/>
+      <c r="BN1" s="51"/>
+      <c r="BO1" s="51"/>
+      <c r="BP1" s="51"/>
+      <c r="BQ1" s="51"/>
+      <c r="BR1" s="51"/>
+      <c r="BS1" s="51"/>
+      <c r="BT1" s="51"/>
+      <c r="BU1" s="51"/>
+      <c r="BV1" s="51"/>
+      <c r="BW1" s="51"/>
+      <c r="BX1" s="51"/>
+      <c r="BY1" s="51"/>
+      <c r="BZ1" s="51"/>
+      <c r="CA1" s="51"/>
+      <c r="CB1" s="51"/>
+      <c r="CC1" s="51"/>
+      <c r="CD1" s="51"/>
+      <c r="CE1" s="51"/>
+      <c r="CF1" s="51"/>
+      <c r="CG1" s="51"/>
+      <c r="CH1" s="51"/>
+      <c r="CI1" s="51"/>
+      <c r="CJ1" s="51"/>
+      <c r="CK1" s="51"/>
+      <c r="CL1" s="51"/>
+      <c r="CM1" s="51"/>
+      <c r="CN1" s="51"/>
+      <c r="CO1" s="51"/>
+      <c r="CP1" s="51"/>
+      <c r="CQ1" s="51"/>
+      <c r="CR1" s="51"/>
+      <c r="CS1" s="51"/>
+      <c r="CT1" s="51"/>
+      <c r="CU1" s="51"/>
+      <c r="CV1" s="51"/>
+      <c r="CW1" s="51"/>
+      <c r="CX1" s="51"/>
+      <c r="CY1" s="51"/>
       <c r="CZ1" s="11"/>
     </row>
     <row r="2" spans="1:104" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="51" t="s">
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="51" t="s">
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="52"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="51" t="s">
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="52"/>
-      <c r="AD2" s="52"/>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="52"/>
-      <c r="AG2" s="52"/>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="51" t="s">
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="53"/>
+      <c r="AF2" s="53"/>
+      <c r="AG2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="AJ2" s="52"/>
-      <c r="AK2" s="52"/>
-      <c r="AL2" s="52"/>
-      <c r="AM2" s="52"/>
-      <c r="AN2" s="52"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="51" t="s">
+      <c r="AJ2" s="53"/>
+      <c r="AK2" s="53"/>
+      <c r="AL2" s="53"/>
+      <c r="AM2" s="53"/>
+      <c r="AN2" s="53"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="AQ2" s="52"/>
-      <c r="AR2" s="52"/>
-      <c r="AS2" s="52"/>
-      <c r="AT2" s="52"/>
-      <c r="AU2" s="52"/>
-      <c r="AV2" s="53"/>
-      <c r="AW2" s="51" t="s">
+      <c r="AQ2" s="53"/>
+      <c r="AR2" s="53"/>
+      <c r="AS2" s="53"/>
+      <c r="AT2" s="53"/>
+      <c r="AU2" s="53"/>
+      <c r="AV2" s="54"/>
+      <c r="AW2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="AX2" s="52"/>
-      <c r="AY2" s="52"/>
-      <c r="AZ2" s="52"/>
-      <c r="BA2" s="52"/>
-      <c r="BB2" s="52"/>
-      <c r="BC2" s="53"/>
-      <c r="BD2" s="51" t="s">
+      <c r="AX2" s="53"/>
+      <c r="AY2" s="53"/>
+      <c r="AZ2" s="53"/>
+      <c r="BA2" s="53"/>
+      <c r="BB2" s="53"/>
+      <c r="BC2" s="54"/>
+      <c r="BD2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="BE2" s="52"/>
-      <c r="BF2" s="52"/>
-      <c r="BG2" s="52"/>
-      <c r="BH2" s="52"/>
-      <c r="BI2" s="52"/>
-      <c r="BJ2" s="53"/>
-      <c r="BK2" s="51" t="s">
+      <c r="BE2" s="53"/>
+      <c r="BF2" s="53"/>
+      <c r="BG2" s="53"/>
+      <c r="BH2" s="53"/>
+      <c r="BI2" s="53"/>
+      <c r="BJ2" s="54"/>
+      <c r="BK2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="BL2" s="52"/>
-      <c r="BM2" s="52"/>
-      <c r="BN2" s="52"/>
-      <c r="BO2" s="52"/>
-      <c r="BP2" s="52"/>
-      <c r="BQ2" s="53"/>
-      <c r="BR2" s="51" t="s">
+      <c r="BL2" s="53"/>
+      <c r="BM2" s="53"/>
+      <c r="BN2" s="53"/>
+      <c r="BO2" s="53"/>
+      <c r="BP2" s="53"/>
+      <c r="BQ2" s="54"/>
+      <c r="BR2" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="BS2" s="52"/>
-      <c r="BT2" s="52"/>
-      <c r="BU2" s="52"/>
-      <c r="BV2" s="52"/>
-      <c r="BW2" s="52"/>
-      <c r="BX2" s="53"/>
-      <c r="BY2" s="51" t="s">
+      <c r="BS2" s="53"/>
+      <c r="BT2" s="53"/>
+      <c r="BU2" s="53"/>
+      <c r="BV2" s="53"/>
+      <c r="BW2" s="53"/>
+      <c r="BX2" s="54"/>
+      <c r="BY2" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="BZ2" s="52"/>
-      <c r="CA2" s="52"/>
-      <c r="CB2" s="52"/>
-      <c r="CC2" s="52"/>
-      <c r="CD2" s="52"/>
-      <c r="CE2" s="53"/>
-      <c r="CF2" s="51" t="s">
+      <c r="BZ2" s="53"/>
+      <c r="CA2" s="53"/>
+      <c r="CB2" s="53"/>
+      <c r="CC2" s="53"/>
+      <c r="CD2" s="53"/>
+      <c r="CE2" s="54"/>
+      <c r="CF2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="CG2" s="52"/>
-      <c r="CH2" s="52"/>
-      <c r="CI2" s="52"/>
-      <c r="CJ2" s="52"/>
-      <c r="CK2" s="52"/>
-      <c r="CL2" s="53"/>
-      <c r="CM2" s="51" t="s">
+      <c r="CG2" s="53"/>
+      <c r="CH2" s="53"/>
+      <c r="CI2" s="53"/>
+      <c r="CJ2" s="53"/>
+      <c r="CK2" s="53"/>
+      <c r="CL2" s="54"/>
+      <c r="CM2" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="CN2" s="52"/>
-      <c r="CO2" s="52"/>
-      <c r="CP2" s="52"/>
-      <c r="CQ2" s="52"/>
-      <c r="CR2" s="52"/>
-      <c r="CS2" s="53"/>
-      <c r="CT2" s="51" t="s">
+      <c r="CN2" s="53"/>
+      <c r="CO2" s="53"/>
+      <c r="CP2" s="53"/>
+      <c r="CQ2" s="53"/>
+      <c r="CR2" s="53"/>
+      <c r="CS2" s="54"/>
+      <c r="CT2" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="CU2" s="52"/>
-      <c r="CV2" s="52"/>
-      <c r="CW2" s="52"/>
-      <c r="CX2" s="52"/>
-      <c r="CY2" s="52"/>
-      <c r="CZ2" s="53"/>
+      <c r="CU2" s="53"/>
+      <c r="CV2" s="53"/>
+      <c r="CW2" s="53"/>
+      <c r="CX2" s="53"/>
+      <c r="CY2" s="53"/>
+      <c r="CZ2" s="54"/>
     </row>
     <row r="3" spans="1:104" x14ac:dyDescent="0.25">
-      <c r="G3" s="59">
+      <c r="G3" s="55">
         <f>G5</f>
         <v>42107</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="54">
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="59">
         <f>N5</f>
         <v>42114</v>
       </c>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="54">
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="59">
         <f>U5</f>
         <v>42121</v>
       </c>
-      <c r="V3" s="55"/>
-      <c r="W3" s="55"/>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="55"/>
-      <c r="Z3" s="55"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="54">
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="57"/>
+      <c r="AB3" s="59">
         <f>AB5</f>
         <v>42128</v>
       </c>
-      <c r="AC3" s="55"/>
-      <c r="AD3" s="55"/>
-      <c r="AE3" s="55"/>
-      <c r="AF3" s="55"/>
-      <c r="AG3" s="55"/>
-      <c r="AH3" s="56"/>
-      <c r="AI3" s="54">
+      <c r="AC3" s="56"/>
+      <c r="AD3" s="56"/>
+      <c r="AE3" s="56"/>
+      <c r="AF3" s="56"/>
+      <c r="AG3" s="56"/>
+      <c r="AH3" s="57"/>
+      <c r="AI3" s="59">
         <f>AI5</f>
         <v>42135</v>
       </c>
-      <c r="AJ3" s="55"/>
-      <c r="AK3" s="55"/>
-      <c r="AL3" s="55"/>
-      <c r="AM3" s="55"/>
-      <c r="AN3" s="55"/>
-      <c r="AO3" s="56"/>
-      <c r="AP3" s="54">
+      <c r="AJ3" s="56"/>
+      <c r="AK3" s="56"/>
+      <c r="AL3" s="56"/>
+      <c r="AM3" s="56"/>
+      <c r="AN3" s="56"/>
+      <c r="AO3" s="57"/>
+      <c r="AP3" s="59">
         <f>AP5</f>
         <v>42142</v>
       </c>
-      <c r="AQ3" s="55"/>
-      <c r="AR3" s="55"/>
-      <c r="AS3" s="55"/>
-      <c r="AT3" s="55"/>
-      <c r="AU3" s="55"/>
-      <c r="AV3" s="56"/>
-      <c r="AW3" s="54">
+      <c r="AQ3" s="56"/>
+      <c r="AR3" s="56"/>
+      <c r="AS3" s="56"/>
+      <c r="AT3" s="56"/>
+      <c r="AU3" s="56"/>
+      <c r="AV3" s="57"/>
+      <c r="AW3" s="59">
         <f t="shared" ref="AW3" si="0">AW5</f>
         <v>42149</v>
       </c>
-      <c r="AX3" s="55"/>
-      <c r="AY3" s="55"/>
-      <c r="AZ3" s="55"/>
-      <c r="BA3" s="55"/>
-      <c r="BB3" s="55"/>
-      <c r="BC3" s="56"/>
-      <c r="BD3" s="54">
+      <c r="AX3" s="56"/>
+      <c r="AY3" s="56"/>
+      <c r="AZ3" s="56"/>
+      <c r="BA3" s="56"/>
+      <c r="BB3" s="56"/>
+      <c r="BC3" s="57"/>
+      <c r="BD3" s="59">
         <f t="shared" ref="BD3" si="1">BD5</f>
         <v>42156</v>
       </c>
-      <c r="BE3" s="55"/>
-      <c r="BF3" s="55"/>
-      <c r="BG3" s="55"/>
-      <c r="BH3" s="55"/>
-      <c r="BI3" s="55"/>
-      <c r="BJ3" s="56"/>
-      <c r="BK3" s="54">
+      <c r="BE3" s="56"/>
+      <c r="BF3" s="56"/>
+      <c r="BG3" s="56"/>
+      <c r="BH3" s="56"/>
+      <c r="BI3" s="56"/>
+      <c r="BJ3" s="57"/>
+      <c r="BK3" s="59">
         <f t="shared" ref="BK3" si="2">BK5</f>
         <v>42163</v>
       </c>
-      <c r="BL3" s="55"/>
-      <c r="BM3" s="55"/>
-      <c r="BN3" s="55"/>
-      <c r="BO3" s="55"/>
-      <c r="BP3" s="55"/>
-      <c r="BQ3" s="56"/>
-      <c r="BR3" s="54">
+      <c r="BL3" s="56"/>
+      <c r="BM3" s="56"/>
+      <c r="BN3" s="56"/>
+      <c r="BO3" s="56"/>
+      <c r="BP3" s="56"/>
+      <c r="BQ3" s="57"/>
+      <c r="BR3" s="59">
         <f t="shared" ref="BR3" si="3">BR5</f>
         <v>42170</v>
       </c>
-      <c r="BS3" s="55"/>
-      <c r="BT3" s="55"/>
-      <c r="BU3" s="55"/>
-      <c r="BV3" s="55"/>
-      <c r="BW3" s="55"/>
-      <c r="BX3" s="56"/>
-      <c r="BY3" s="54">
+      <c r="BS3" s="56"/>
+      <c r="BT3" s="56"/>
+      <c r="BU3" s="56"/>
+      <c r="BV3" s="56"/>
+      <c r="BW3" s="56"/>
+      <c r="BX3" s="57"/>
+      <c r="BY3" s="59">
         <f t="shared" ref="BY3" si="4">BY5</f>
         <v>42177</v>
       </c>
-      <c r="BZ3" s="55"/>
-      <c r="CA3" s="55"/>
-      <c r="CB3" s="55"/>
-      <c r="CC3" s="55"/>
-      <c r="CD3" s="55"/>
-      <c r="CE3" s="56"/>
-      <c r="CF3" s="54">
+      <c r="BZ3" s="56"/>
+      <c r="CA3" s="56"/>
+      <c r="CB3" s="56"/>
+      <c r="CC3" s="56"/>
+      <c r="CD3" s="56"/>
+      <c r="CE3" s="57"/>
+      <c r="CF3" s="59">
         <f t="shared" ref="CF3" si="5">CF5</f>
         <v>42184</v>
       </c>
-      <c r="CG3" s="55"/>
-      <c r="CH3" s="55"/>
-      <c r="CI3" s="55"/>
-      <c r="CJ3" s="55"/>
-      <c r="CK3" s="55"/>
-      <c r="CL3" s="56"/>
-      <c r="CM3" s="54">
+      <c r="CG3" s="56"/>
+      <c r="CH3" s="56"/>
+      <c r="CI3" s="56"/>
+      <c r="CJ3" s="56"/>
+      <c r="CK3" s="56"/>
+      <c r="CL3" s="57"/>
+      <c r="CM3" s="59">
         <f t="shared" ref="CM3" si="6">CM5</f>
         <v>42191</v>
       </c>
-      <c r="CN3" s="55"/>
-      <c r="CO3" s="55"/>
-      <c r="CP3" s="55"/>
-      <c r="CQ3" s="55"/>
-      <c r="CR3" s="55"/>
-      <c r="CS3" s="56"/>
-      <c r="CT3" s="54">
+      <c r="CN3" s="56"/>
+      <c r="CO3" s="56"/>
+      <c r="CP3" s="56"/>
+      <c r="CQ3" s="56"/>
+      <c r="CR3" s="56"/>
+      <c r="CS3" s="57"/>
+      <c r="CT3" s="59">
         <f t="shared" ref="CT3" si="7">CT5</f>
         <v>42198</v>
       </c>
-      <c r="CU3" s="55"/>
-      <c r="CV3" s="55"/>
-      <c r="CW3" s="55"/>
-      <c r="CX3" s="55"/>
-      <c r="CY3" s="55"/>
-      <c r="CZ3" s="56"/>
+      <c r="CU3" s="56"/>
+      <c r="CV3" s="56"/>
+      <c r="CW3" s="56"/>
+      <c r="CX3" s="56"/>
+      <c r="CY3" s="56"/>
+      <c r="CZ3" s="57"/>
     </row>
     <row r="4" spans="1:104" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
@@ -10235,7 +10184,7 @@
         <v>42204</v>
       </c>
     </row>
-    <row r="6" spans="1:104" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="str">
         <f>IF('Milestones + Packages'!B3&lt;&gt; "",'Milestones + Packages'!B3,"")</f>
         <v>Brainstorming phase</v>
@@ -22155,6 +22104,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="CT2:CZ2"/>
+    <mergeCell ref="CM3:CS3"/>
+    <mergeCell ref="CT3:CZ3"/>
+    <mergeCell ref="BY2:CE2"/>
+    <mergeCell ref="CF2:CL2"/>
+    <mergeCell ref="BY3:CE3"/>
+    <mergeCell ref="CF3:CL3"/>
+    <mergeCell ref="CM2:CS2"/>
+    <mergeCell ref="BD3:BJ3"/>
+    <mergeCell ref="BK2:BQ2"/>
+    <mergeCell ref="BR2:BX2"/>
+    <mergeCell ref="BK3:BQ3"/>
+    <mergeCell ref="BR3:BX3"/>
     <mergeCell ref="A1:CY1"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="G3:M3"/>
@@ -22171,22 +22133,9 @@
     <mergeCell ref="AI3:AO3"/>
     <mergeCell ref="AP3:AV3"/>
     <mergeCell ref="AW3:BC3"/>
-    <mergeCell ref="BD3:BJ3"/>
-    <mergeCell ref="BK2:BQ2"/>
-    <mergeCell ref="BR2:BX2"/>
-    <mergeCell ref="BK3:BQ3"/>
-    <mergeCell ref="BR3:BX3"/>
-    <mergeCell ref="CT2:CZ2"/>
-    <mergeCell ref="CM3:CS3"/>
-    <mergeCell ref="CT3:CZ3"/>
-    <mergeCell ref="BY2:CE2"/>
-    <mergeCell ref="CF2:CL2"/>
-    <mergeCell ref="BY3:CE3"/>
-    <mergeCell ref="CF3:CL3"/>
-    <mergeCell ref="CM2:CS2"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:CW300">
-    <cfRule type="expression" dxfId="21" priority="77">
+    <cfRule type="expression" dxfId="14" priority="77">
       <formula>NOT(ISNA(VLOOKUP(G$5,$F:$F,1,FALSE)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45374,15 +45323,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" customWidth="1"/>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" customWidth="1"/>
     <col min="4" max="4" width="46.140625" customWidth="1"/>
@@ -45417,26 +45366,73 @@
       </c>
       <c r="H3">
         <f>SUM(Table1345[Time Spent (hours)])</f>
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>157</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added worked hours, cleaned up folder structure
</commit_message>
<xml_diff>
--- a/Project Schedule.xlsx
+++ b/Project Schedule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fin Bauer\Documents\Case Studies\CaseStudiesMachineLearning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\Git\CaseStudiesMachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="9570" tabRatio="842" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="9570" tabRatio="842" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Some Hints and Explanations" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="188">
   <si>
     <t>Typ</t>
   </si>
@@ -606,6 +606,15 @@
   <si>
     <t>Special lecture</t>
   </si>
+  <si>
+    <t>6.9.</t>
+  </si>
+  <si>
+    <t>8.9.</t>
+  </si>
+  <si>
+    <t>10.9.</t>
+  </si>
 </sst>
 </file>
 
@@ -1016,7 +1025,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1025,7 +1039,7 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="15" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="12" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1034,23 +1048,18 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="15" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift 3" xfId="2" builtinId="18"/>
-    <cellStyle name="Überschrift 4" xfId="3" builtinId="19"/>
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="3" builtinId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
     <dxf>
@@ -1605,7 +1614,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="111.5703125" customWidth="1"/>
   </cols>
@@ -1709,7 +1718,7 @@
       <selection activeCell="L36" sqref="A36:L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="21" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="23" customWidth="1"/>
@@ -4742,7 +4751,7 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="21" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="23" customWidth="1"/>
@@ -9215,7 +9224,7 @@
       <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.42578125" style="13" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
@@ -9255,385 +9264,385 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:104" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="57"/>
-      <c r="AD1" s="57"/>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="57"/>
-      <c r="AG1" s="57"/>
-      <c r="AH1" s="57"/>
-      <c r="AI1" s="57"/>
-      <c r="AJ1" s="57"/>
-      <c r="AK1" s="57"/>
-      <c r="AL1" s="57"/>
-      <c r="AM1" s="57"/>
-      <c r="AN1" s="57"/>
-      <c r="AO1" s="57"/>
-      <c r="AP1" s="57"/>
-      <c r="AQ1" s="57"/>
-      <c r="AR1" s="57"/>
-      <c r="AS1" s="57"/>
-      <c r="AT1" s="57"/>
-      <c r="AU1" s="57"/>
-      <c r="AV1" s="57"/>
-      <c r="AW1" s="57"/>
-      <c r="AX1" s="57"/>
-      <c r="AY1" s="57"/>
-      <c r="AZ1" s="57"/>
-      <c r="BA1" s="57"/>
-      <c r="BB1" s="57"/>
-      <c r="BC1" s="57"/>
-      <c r="BD1" s="57"/>
-      <c r="BE1" s="57"/>
-      <c r="BF1" s="57"/>
-      <c r="BG1" s="57"/>
-      <c r="BH1" s="57"/>
-      <c r="BI1" s="57"/>
-      <c r="BJ1" s="57"/>
-      <c r="BK1" s="57"/>
-      <c r="BL1" s="57"/>
-      <c r="BM1" s="57"/>
-      <c r="BN1" s="57"/>
-      <c r="BO1" s="57"/>
-      <c r="BP1" s="57"/>
-      <c r="BQ1" s="57"/>
-      <c r="BR1" s="57"/>
-      <c r="BS1" s="57"/>
-      <c r="BT1" s="57"/>
-      <c r="BU1" s="57"/>
-      <c r="BV1" s="57"/>
-      <c r="BW1" s="57"/>
-      <c r="BX1" s="57"/>
-      <c r="BY1" s="57"/>
-      <c r="BZ1" s="57"/>
-      <c r="CA1" s="57"/>
-      <c r="CB1" s="57"/>
-      <c r="CC1" s="57"/>
-      <c r="CD1" s="57"/>
-      <c r="CE1" s="57"/>
-      <c r="CF1" s="57"/>
-      <c r="CG1" s="57"/>
-      <c r="CH1" s="57"/>
-      <c r="CI1" s="57"/>
-      <c r="CJ1" s="57"/>
-      <c r="CK1" s="57"/>
-      <c r="CL1" s="57"/>
-      <c r="CM1" s="57"/>
-      <c r="CN1" s="57"/>
-      <c r="CO1" s="57"/>
-      <c r="CP1" s="57"/>
-      <c r="CQ1" s="57"/>
-      <c r="CR1" s="57"/>
-      <c r="CS1" s="57"/>
-      <c r="CT1" s="57"/>
-      <c r="CU1" s="57"/>
-      <c r="CV1" s="57"/>
-      <c r="CW1" s="57"/>
-      <c r="CX1" s="57"/>
-      <c r="CY1" s="57"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="53"/>
+      <c r="AL1" s="53"/>
+      <c r="AM1" s="53"/>
+      <c r="AN1" s="53"/>
+      <c r="AO1" s="53"/>
+      <c r="AP1" s="53"/>
+      <c r="AQ1" s="53"/>
+      <c r="AR1" s="53"/>
+      <c r="AS1" s="53"/>
+      <c r="AT1" s="53"/>
+      <c r="AU1" s="53"/>
+      <c r="AV1" s="53"/>
+      <c r="AW1" s="53"/>
+      <c r="AX1" s="53"/>
+      <c r="AY1" s="53"/>
+      <c r="AZ1" s="53"/>
+      <c r="BA1" s="53"/>
+      <c r="BB1" s="53"/>
+      <c r="BC1" s="53"/>
+      <c r="BD1" s="53"/>
+      <c r="BE1" s="53"/>
+      <c r="BF1" s="53"/>
+      <c r="BG1" s="53"/>
+      <c r="BH1" s="53"/>
+      <c r="BI1" s="53"/>
+      <c r="BJ1" s="53"/>
+      <c r="BK1" s="53"/>
+      <c r="BL1" s="53"/>
+      <c r="BM1" s="53"/>
+      <c r="BN1" s="53"/>
+      <c r="BO1" s="53"/>
+      <c r="BP1" s="53"/>
+      <c r="BQ1" s="53"/>
+      <c r="BR1" s="53"/>
+      <c r="BS1" s="53"/>
+      <c r="BT1" s="53"/>
+      <c r="BU1" s="53"/>
+      <c r="BV1" s="53"/>
+      <c r="BW1" s="53"/>
+      <c r="BX1" s="53"/>
+      <c r="BY1" s="53"/>
+      <c r="BZ1" s="53"/>
+      <c r="CA1" s="53"/>
+      <c r="CB1" s="53"/>
+      <c r="CC1" s="53"/>
+      <c r="CD1" s="53"/>
+      <c r="CE1" s="53"/>
+      <c r="CF1" s="53"/>
+      <c r="CG1" s="53"/>
+      <c r="CH1" s="53"/>
+      <c r="CI1" s="53"/>
+      <c r="CJ1" s="53"/>
+      <c r="CK1" s="53"/>
+      <c r="CL1" s="53"/>
+      <c r="CM1" s="53"/>
+      <c r="CN1" s="53"/>
+      <c r="CO1" s="53"/>
+      <c r="CP1" s="53"/>
+      <c r="CQ1" s="53"/>
+      <c r="CR1" s="53"/>
+      <c r="CS1" s="53"/>
+      <c r="CT1" s="53"/>
+      <c r="CU1" s="53"/>
+      <c r="CV1" s="53"/>
+      <c r="CW1" s="53"/>
+      <c r="CX1" s="53"/>
+      <c r="CY1" s="53"/>
       <c r="CZ1" s="11"/>
     </row>
     <row r="2" spans="1:104" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="51" t="s">
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="51" t="s">
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="52"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="51" t="s">
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="52"/>
-      <c r="AD2" s="52"/>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="52"/>
-      <c r="AG2" s="52"/>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="51" t="s">
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="55"/>
+      <c r="AE2" s="55"/>
+      <c r="AF2" s="55"/>
+      <c r="AG2" s="55"/>
+      <c r="AH2" s="56"/>
+      <c r="AI2" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="AJ2" s="52"/>
-      <c r="AK2" s="52"/>
-      <c r="AL2" s="52"/>
-      <c r="AM2" s="52"/>
-      <c r="AN2" s="52"/>
-      <c r="AO2" s="53"/>
-      <c r="AP2" s="51" t="s">
+      <c r="AJ2" s="55"/>
+      <c r="AK2" s="55"/>
+      <c r="AL2" s="55"/>
+      <c r="AM2" s="55"/>
+      <c r="AN2" s="55"/>
+      <c r="AO2" s="56"/>
+      <c r="AP2" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="AQ2" s="52"/>
-      <c r="AR2" s="52"/>
-      <c r="AS2" s="52"/>
-      <c r="AT2" s="52"/>
-      <c r="AU2" s="52"/>
-      <c r="AV2" s="53"/>
-      <c r="AW2" s="51" t="s">
+      <c r="AQ2" s="55"/>
+      <c r="AR2" s="55"/>
+      <c r="AS2" s="55"/>
+      <c r="AT2" s="55"/>
+      <c r="AU2" s="55"/>
+      <c r="AV2" s="56"/>
+      <c r="AW2" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="AX2" s="52"/>
-      <c r="AY2" s="52"/>
-      <c r="AZ2" s="52"/>
-      <c r="BA2" s="52"/>
-      <c r="BB2" s="52"/>
-      <c r="BC2" s="53"/>
-      <c r="BD2" s="51" t="s">
+      <c r="AX2" s="55"/>
+      <c r="AY2" s="55"/>
+      <c r="AZ2" s="55"/>
+      <c r="BA2" s="55"/>
+      <c r="BB2" s="55"/>
+      <c r="BC2" s="56"/>
+      <c r="BD2" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="BE2" s="52"/>
-      <c r="BF2" s="52"/>
-      <c r="BG2" s="52"/>
-      <c r="BH2" s="52"/>
-      <c r="BI2" s="52"/>
-      <c r="BJ2" s="53"/>
-      <c r="BK2" s="51" t="s">
+      <c r="BE2" s="55"/>
+      <c r="BF2" s="55"/>
+      <c r="BG2" s="55"/>
+      <c r="BH2" s="55"/>
+      <c r="BI2" s="55"/>
+      <c r="BJ2" s="56"/>
+      <c r="BK2" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="BL2" s="52"/>
-      <c r="BM2" s="52"/>
-      <c r="BN2" s="52"/>
-      <c r="BO2" s="52"/>
-      <c r="BP2" s="52"/>
-      <c r="BQ2" s="53"/>
-      <c r="BR2" s="51" t="s">
+      <c r="BL2" s="55"/>
+      <c r="BM2" s="55"/>
+      <c r="BN2" s="55"/>
+      <c r="BO2" s="55"/>
+      <c r="BP2" s="55"/>
+      <c r="BQ2" s="56"/>
+      <c r="BR2" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="BS2" s="52"/>
-      <c r="BT2" s="52"/>
-      <c r="BU2" s="52"/>
-      <c r="BV2" s="52"/>
-      <c r="BW2" s="52"/>
-      <c r="BX2" s="53"/>
-      <c r="BY2" s="51" t="s">
+      <c r="BS2" s="55"/>
+      <c r="BT2" s="55"/>
+      <c r="BU2" s="55"/>
+      <c r="BV2" s="55"/>
+      <c r="BW2" s="55"/>
+      <c r="BX2" s="56"/>
+      <c r="BY2" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="BZ2" s="52"/>
-      <c r="CA2" s="52"/>
-      <c r="CB2" s="52"/>
-      <c r="CC2" s="52"/>
-      <c r="CD2" s="52"/>
-      <c r="CE2" s="53"/>
-      <c r="CF2" s="51" t="s">
+      <c r="BZ2" s="55"/>
+      <c r="CA2" s="55"/>
+      <c r="CB2" s="55"/>
+      <c r="CC2" s="55"/>
+      <c r="CD2" s="55"/>
+      <c r="CE2" s="56"/>
+      <c r="CF2" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="CG2" s="52"/>
-      <c r="CH2" s="52"/>
-      <c r="CI2" s="52"/>
-      <c r="CJ2" s="52"/>
-      <c r="CK2" s="52"/>
-      <c r="CL2" s="53"/>
-      <c r="CM2" s="51" t="s">
+      <c r="CG2" s="55"/>
+      <c r="CH2" s="55"/>
+      <c r="CI2" s="55"/>
+      <c r="CJ2" s="55"/>
+      <c r="CK2" s="55"/>
+      <c r="CL2" s="56"/>
+      <c r="CM2" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="CN2" s="52"/>
-      <c r="CO2" s="52"/>
-      <c r="CP2" s="52"/>
-      <c r="CQ2" s="52"/>
-      <c r="CR2" s="52"/>
-      <c r="CS2" s="53"/>
-      <c r="CT2" s="51" t="s">
+      <c r="CN2" s="55"/>
+      <c r="CO2" s="55"/>
+      <c r="CP2" s="55"/>
+      <c r="CQ2" s="55"/>
+      <c r="CR2" s="55"/>
+      <c r="CS2" s="56"/>
+      <c r="CT2" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="CU2" s="52"/>
-      <c r="CV2" s="52"/>
-      <c r="CW2" s="52"/>
-      <c r="CX2" s="52"/>
-      <c r="CY2" s="52"/>
-      <c r="CZ2" s="53"/>
+      <c r="CU2" s="55"/>
+      <c r="CV2" s="55"/>
+      <c r="CW2" s="55"/>
+      <c r="CX2" s="55"/>
+      <c r="CY2" s="55"/>
+      <c r="CZ2" s="56"/>
     </row>
     <row r="3" spans="1:104" x14ac:dyDescent="0.25">
-      <c r="G3" s="59">
+      <c r="G3" s="57">
         <f>G5</f>
         <v>42107</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="54">
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="61">
         <f>N5</f>
         <v>42114</v>
       </c>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="54">
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="61">
         <f>U5</f>
         <v>42121</v>
       </c>
-      <c r="V3" s="55"/>
-      <c r="W3" s="55"/>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="55"/>
-      <c r="Z3" s="55"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="54">
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="61">
         <f>AB5</f>
         <v>42128</v>
       </c>
-      <c r="AC3" s="55"/>
-      <c r="AD3" s="55"/>
-      <c r="AE3" s="55"/>
-      <c r="AF3" s="55"/>
-      <c r="AG3" s="55"/>
-      <c r="AH3" s="56"/>
-      <c r="AI3" s="54">
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58"/>
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="59"/>
+      <c r="AI3" s="61">
         <f>AI5</f>
         <v>42135</v>
       </c>
-      <c r="AJ3" s="55"/>
-      <c r="AK3" s="55"/>
-      <c r="AL3" s="55"/>
-      <c r="AM3" s="55"/>
-      <c r="AN3" s="55"/>
-      <c r="AO3" s="56"/>
-      <c r="AP3" s="54">
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58"/>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="58"/>
+      <c r="AN3" s="58"/>
+      <c r="AO3" s="59"/>
+      <c r="AP3" s="61">
         <f>AP5</f>
         <v>42142</v>
       </c>
-      <c r="AQ3" s="55"/>
-      <c r="AR3" s="55"/>
-      <c r="AS3" s="55"/>
-      <c r="AT3" s="55"/>
-      <c r="AU3" s="55"/>
-      <c r="AV3" s="56"/>
-      <c r="AW3" s="54">
+      <c r="AQ3" s="58"/>
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58"/>
+      <c r="AU3" s="58"/>
+      <c r="AV3" s="59"/>
+      <c r="AW3" s="61">
         <f t="shared" ref="AW3" si="0">AW5</f>
         <v>42149</v>
       </c>
-      <c r="AX3" s="55"/>
-      <c r="AY3" s="55"/>
-      <c r="AZ3" s="55"/>
-      <c r="BA3" s="55"/>
-      <c r="BB3" s="55"/>
-      <c r="BC3" s="56"/>
-      <c r="BD3" s="54">
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="58"/>
+      <c r="AZ3" s="58"/>
+      <c r="BA3" s="58"/>
+      <c r="BB3" s="58"/>
+      <c r="BC3" s="59"/>
+      <c r="BD3" s="61">
         <f t="shared" ref="BD3" si="1">BD5</f>
         <v>42156</v>
       </c>
-      <c r="BE3" s="55"/>
-      <c r="BF3" s="55"/>
-      <c r="BG3" s="55"/>
-      <c r="BH3" s="55"/>
-      <c r="BI3" s="55"/>
-      <c r="BJ3" s="56"/>
-      <c r="BK3" s="54">
+      <c r="BE3" s="58"/>
+      <c r="BF3" s="58"/>
+      <c r="BG3" s="58"/>
+      <c r="BH3" s="58"/>
+      <c r="BI3" s="58"/>
+      <c r="BJ3" s="59"/>
+      <c r="BK3" s="61">
         <f t="shared" ref="BK3" si="2">BK5</f>
         <v>42163</v>
       </c>
-      <c r="BL3" s="55"/>
-      <c r="BM3" s="55"/>
-      <c r="BN3" s="55"/>
-      <c r="BO3" s="55"/>
-      <c r="BP3" s="55"/>
-      <c r="BQ3" s="56"/>
-      <c r="BR3" s="54">
+      <c r="BL3" s="58"/>
+      <c r="BM3" s="58"/>
+      <c r="BN3" s="58"/>
+      <c r="BO3" s="58"/>
+      <c r="BP3" s="58"/>
+      <c r="BQ3" s="59"/>
+      <c r="BR3" s="61">
         <f t="shared" ref="BR3" si="3">BR5</f>
         <v>42170</v>
       </c>
-      <c r="BS3" s="55"/>
-      <c r="BT3" s="55"/>
-      <c r="BU3" s="55"/>
-      <c r="BV3" s="55"/>
-      <c r="BW3" s="55"/>
-      <c r="BX3" s="56"/>
-      <c r="BY3" s="54">
+      <c r="BS3" s="58"/>
+      <c r="BT3" s="58"/>
+      <c r="BU3" s="58"/>
+      <c r="BV3" s="58"/>
+      <c r="BW3" s="58"/>
+      <c r="BX3" s="59"/>
+      <c r="BY3" s="61">
         <f t="shared" ref="BY3" si="4">BY5</f>
         <v>42177</v>
       </c>
-      <c r="BZ3" s="55"/>
-      <c r="CA3" s="55"/>
-      <c r="CB3" s="55"/>
-      <c r="CC3" s="55"/>
-      <c r="CD3" s="55"/>
-      <c r="CE3" s="56"/>
-      <c r="CF3" s="54">
+      <c r="BZ3" s="58"/>
+      <c r="CA3" s="58"/>
+      <c r="CB3" s="58"/>
+      <c r="CC3" s="58"/>
+      <c r="CD3" s="58"/>
+      <c r="CE3" s="59"/>
+      <c r="CF3" s="61">
         <f t="shared" ref="CF3" si="5">CF5</f>
         <v>42184</v>
       </c>
-      <c r="CG3" s="55"/>
-      <c r="CH3" s="55"/>
-      <c r="CI3" s="55"/>
-      <c r="CJ3" s="55"/>
-      <c r="CK3" s="55"/>
-      <c r="CL3" s="56"/>
-      <c r="CM3" s="54">
+      <c r="CG3" s="58"/>
+      <c r="CH3" s="58"/>
+      <c r="CI3" s="58"/>
+      <c r="CJ3" s="58"/>
+      <c r="CK3" s="58"/>
+      <c r="CL3" s="59"/>
+      <c r="CM3" s="61">
         <f t="shared" ref="CM3" si="6">CM5</f>
         <v>42191</v>
       </c>
-      <c r="CN3" s="55"/>
-      <c r="CO3" s="55"/>
-      <c r="CP3" s="55"/>
-      <c r="CQ3" s="55"/>
-      <c r="CR3" s="55"/>
-      <c r="CS3" s="56"/>
-      <c r="CT3" s="54">
+      <c r="CN3" s="58"/>
+      <c r="CO3" s="58"/>
+      <c r="CP3" s="58"/>
+      <c r="CQ3" s="58"/>
+      <c r="CR3" s="58"/>
+      <c r="CS3" s="59"/>
+      <c r="CT3" s="61">
         <f t="shared" ref="CT3" si="7">CT5</f>
         <v>42198</v>
       </c>
-      <c r="CU3" s="55"/>
-      <c r="CV3" s="55"/>
-      <c r="CW3" s="55"/>
-      <c r="CX3" s="55"/>
-      <c r="CY3" s="55"/>
-      <c r="CZ3" s="56"/>
+      <c r="CU3" s="58"/>
+      <c r="CV3" s="58"/>
+      <c r="CW3" s="58"/>
+      <c r="CX3" s="58"/>
+      <c r="CY3" s="58"/>
+      <c r="CZ3" s="59"/>
     </row>
     <row r="4" spans="1:104" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
@@ -22154,6 +22163,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="CT2:CZ2"/>
+    <mergeCell ref="CM3:CS3"/>
+    <mergeCell ref="CT3:CZ3"/>
+    <mergeCell ref="BY2:CE2"/>
+    <mergeCell ref="CF2:CL2"/>
+    <mergeCell ref="BY3:CE3"/>
+    <mergeCell ref="CF3:CL3"/>
+    <mergeCell ref="CM2:CS2"/>
+    <mergeCell ref="BD3:BJ3"/>
+    <mergeCell ref="BK2:BQ2"/>
+    <mergeCell ref="BR2:BX2"/>
+    <mergeCell ref="BK3:BQ3"/>
+    <mergeCell ref="BR3:BX3"/>
     <mergeCell ref="A1:CY1"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="G3:M3"/>
@@ -22170,19 +22192,6 @@
     <mergeCell ref="AI3:AO3"/>
     <mergeCell ref="AP3:AV3"/>
     <mergeCell ref="AW3:BC3"/>
-    <mergeCell ref="BD3:BJ3"/>
-    <mergeCell ref="BK2:BQ2"/>
-    <mergeCell ref="BR2:BX2"/>
-    <mergeCell ref="BK3:BQ3"/>
-    <mergeCell ref="BR3:BX3"/>
-    <mergeCell ref="CT2:CZ2"/>
-    <mergeCell ref="CM3:CS3"/>
-    <mergeCell ref="CT3:CZ3"/>
-    <mergeCell ref="BY2:CE2"/>
-    <mergeCell ref="CF2:CL2"/>
-    <mergeCell ref="BY3:CE3"/>
-    <mergeCell ref="CF3:CL3"/>
-    <mergeCell ref="CM2:CS2"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:CW300">
     <cfRule type="expression" dxfId="14" priority="77">
@@ -22309,7 +22318,7 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
@@ -45104,7 +45113,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -45207,7 +45216,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -45299,7 +45308,7 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -45411,15 +45420,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+    <col min="1" max="1" width="58.42578125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" customWidth="1"/>
     <col min="4" max="4" width="46.140625" customWidth="1"/>
@@ -45454,7 +45463,7 @@
       </c>
       <c r="H3">
         <f>SUM(Table1345[Time Spent (hours)])</f>
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -45554,6 +45563,39 @@
       </c>
       <c r="C12" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13">
+        <v>1.5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15">
+        <v>9.5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -45581,11 +45623,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -45626,79 +45668,79 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="51" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="60">
+      <c r="B4" s="51">
         <v>3</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="51" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="60">
+      <c r="B5" s="51">
         <v>4</v>
       </c>
-      <c r="C5" s="61">
+      <c r="C5" s="52">
         <v>42114</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="51" t="s">
         <v>177</v>
       </c>
-      <c r="B6" s="60">
+      <c r="B6" s="51">
         <v>8</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="51" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="60">
+      <c r="B7" s="51">
         <v>18</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="51" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="60">
+      <c r="B8" s="51">
         <v>2</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="51" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="60">
+      <c r="B9" s="51">
         <v>10</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="51" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="B10" s="60">
+      <c r="B10" s="51">
         <v>2</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="51" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Documentation and hours worked
</commit_message>
<xml_diff>
--- a/Project Schedule.xlsx
+++ b/Project Schedule.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="225">
   <si>
     <t>Typ</t>
   </si>
@@ -726,6 +726,9 @@
   <si>
     <t>SQN implementierung, debugging</t>
   </si>
+  <si>
+    <t>Coding / Reading / Understanding Session bei Fin</t>
+  </si>
 </sst>
 </file>
 
@@ -1135,10 +1138,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1147,7 +1147,7 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="15" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="12" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1156,10 +1156,13 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="15" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9582,385 +9585,385 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:104" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="52"/>
-      <c r="AD1" s="52"/>
-      <c r="AE1" s="52"/>
-      <c r="AF1" s="52"/>
-      <c r="AG1" s="52"/>
-      <c r="AH1" s="52"/>
-      <c r="AI1" s="52"/>
-      <c r="AJ1" s="52"/>
-      <c r="AK1" s="52"/>
-      <c r="AL1" s="52"/>
-      <c r="AM1" s="52"/>
-      <c r="AN1" s="52"/>
-      <c r="AO1" s="52"/>
-      <c r="AP1" s="52"/>
-      <c r="AQ1" s="52"/>
-      <c r="AR1" s="52"/>
-      <c r="AS1" s="52"/>
-      <c r="AT1" s="52"/>
-      <c r="AU1" s="52"/>
-      <c r="AV1" s="52"/>
-      <c r="AW1" s="52"/>
-      <c r="AX1" s="52"/>
-      <c r="AY1" s="52"/>
-      <c r="AZ1" s="52"/>
-      <c r="BA1" s="52"/>
-      <c r="BB1" s="52"/>
-      <c r="BC1" s="52"/>
-      <c r="BD1" s="52"/>
-      <c r="BE1" s="52"/>
-      <c r="BF1" s="52"/>
-      <c r="BG1" s="52"/>
-      <c r="BH1" s="52"/>
-      <c r="BI1" s="52"/>
-      <c r="BJ1" s="52"/>
-      <c r="BK1" s="52"/>
-      <c r="BL1" s="52"/>
-      <c r="BM1" s="52"/>
-      <c r="BN1" s="52"/>
-      <c r="BO1" s="52"/>
-      <c r="BP1" s="52"/>
-      <c r="BQ1" s="52"/>
-      <c r="BR1" s="52"/>
-      <c r="BS1" s="52"/>
-      <c r="BT1" s="52"/>
-      <c r="BU1" s="52"/>
-      <c r="BV1" s="52"/>
-      <c r="BW1" s="52"/>
-      <c r="BX1" s="52"/>
-      <c r="BY1" s="52"/>
-      <c r="BZ1" s="52"/>
-      <c r="CA1" s="52"/>
-      <c r="CB1" s="52"/>
-      <c r="CC1" s="52"/>
-      <c r="CD1" s="52"/>
-      <c r="CE1" s="52"/>
-      <c r="CF1" s="52"/>
-      <c r="CG1" s="52"/>
-      <c r="CH1" s="52"/>
-      <c r="CI1" s="52"/>
-      <c r="CJ1" s="52"/>
-      <c r="CK1" s="52"/>
-      <c r="CL1" s="52"/>
-      <c r="CM1" s="52"/>
-      <c r="CN1" s="52"/>
-      <c r="CO1" s="52"/>
-      <c r="CP1" s="52"/>
-      <c r="CQ1" s="52"/>
-      <c r="CR1" s="52"/>
-      <c r="CS1" s="52"/>
-      <c r="CT1" s="52"/>
-      <c r="CU1" s="52"/>
-      <c r="CV1" s="52"/>
-      <c r="CW1" s="52"/>
-      <c r="CX1" s="52"/>
-      <c r="CY1" s="52"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
+      <c r="AI1" s="58"/>
+      <c r="AJ1" s="58"/>
+      <c r="AK1" s="58"/>
+      <c r="AL1" s="58"/>
+      <c r="AM1" s="58"/>
+      <c r="AN1" s="58"/>
+      <c r="AO1" s="58"/>
+      <c r="AP1" s="58"/>
+      <c r="AQ1" s="58"/>
+      <c r="AR1" s="58"/>
+      <c r="AS1" s="58"/>
+      <c r="AT1" s="58"/>
+      <c r="AU1" s="58"/>
+      <c r="AV1" s="58"/>
+      <c r="AW1" s="58"/>
+      <c r="AX1" s="58"/>
+      <c r="AY1" s="58"/>
+      <c r="AZ1" s="58"/>
+      <c r="BA1" s="58"/>
+      <c r="BB1" s="58"/>
+      <c r="BC1" s="58"/>
+      <c r="BD1" s="58"/>
+      <c r="BE1" s="58"/>
+      <c r="BF1" s="58"/>
+      <c r="BG1" s="58"/>
+      <c r="BH1" s="58"/>
+      <c r="BI1" s="58"/>
+      <c r="BJ1" s="58"/>
+      <c r="BK1" s="58"/>
+      <c r="BL1" s="58"/>
+      <c r="BM1" s="58"/>
+      <c r="BN1" s="58"/>
+      <c r="BO1" s="58"/>
+      <c r="BP1" s="58"/>
+      <c r="BQ1" s="58"/>
+      <c r="BR1" s="58"/>
+      <c r="BS1" s="58"/>
+      <c r="BT1" s="58"/>
+      <c r="BU1" s="58"/>
+      <c r="BV1" s="58"/>
+      <c r="BW1" s="58"/>
+      <c r="BX1" s="58"/>
+      <c r="BY1" s="58"/>
+      <c r="BZ1" s="58"/>
+      <c r="CA1" s="58"/>
+      <c r="CB1" s="58"/>
+      <c r="CC1" s="58"/>
+      <c r="CD1" s="58"/>
+      <c r="CE1" s="58"/>
+      <c r="CF1" s="58"/>
+      <c r="CG1" s="58"/>
+      <c r="CH1" s="58"/>
+      <c r="CI1" s="58"/>
+      <c r="CJ1" s="58"/>
+      <c r="CK1" s="58"/>
+      <c r="CL1" s="58"/>
+      <c r="CM1" s="58"/>
+      <c r="CN1" s="58"/>
+      <c r="CO1" s="58"/>
+      <c r="CP1" s="58"/>
+      <c r="CQ1" s="58"/>
+      <c r="CR1" s="58"/>
+      <c r="CS1" s="58"/>
+      <c r="CT1" s="58"/>
+      <c r="CU1" s="58"/>
+      <c r="CV1" s="58"/>
+      <c r="CW1" s="58"/>
+      <c r="CX1" s="58"/>
+      <c r="CY1" s="58"/>
       <c r="CZ1" s="11"/>
     </row>
     <row r="2" spans="1:104" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="59" t="s">
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="59" t="s">
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="59" t="s">
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
-      <c r="AF2" s="54"/>
-      <c r="AG2" s="54"/>
-      <c r="AH2" s="55"/>
-      <c r="AI2" s="59" t="s">
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="53"/>
+      <c r="AF2" s="53"/>
+      <c r="AG2" s="53"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="55"/>
-      <c r="AP2" s="59" t="s">
+      <c r="AJ2" s="53"/>
+      <c r="AK2" s="53"/>
+      <c r="AL2" s="53"/>
+      <c r="AM2" s="53"/>
+      <c r="AN2" s="53"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="AQ2" s="54"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="54"/>
-      <c r="AT2" s="54"/>
-      <c r="AU2" s="54"/>
-      <c r="AV2" s="55"/>
-      <c r="AW2" s="59" t="s">
+      <c r="AQ2" s="53"/>
+      <c r="AR2" s="53"/>
+      <c r="AS2" s="53"/>
+      <c r="AT2" s="53"/>
+      <c r="AU2" s="53"/>
+      <c r="AV2" s="54"/>
+      <c r="AW2" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="AX2" s="54"/>
-      <c r="AY2" s="54"/>
-      <c r="AZ2" s="54"/>
-      <c r="BA2" s="54"/>
-      <c r="BB2" s="54"/>
-      <c r="BC2" s="55"/>
-      <c r="BD2" s="59" t="s">
+      <c r="AX2" s="53"/>
+      <c r="AY2" s="53"/>
+      <c r="AZ2" s="53"/>
+      <c r="BA2" s="53"/>
+      <c r="BB2" s="53"/>
+      <c r="BC2" s="54"/>
+      <c r="BD2" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="BE2" s="54"/>
-      <c r="BF2" s="54"/>
-      <c r="BG2" s="54"/>
-      <c r="BH2" s="54"/>
-      <c r="BI2" s="54"/>
-      <c r="BJ2" s="55"/>
-      <c r="BK2" s="59" t="s">
+      <c r="BE2" s="53"/>
+      <c r="BF2" s="53"/>
+      <c r="BG2" s="53"/>
+      <c r="BH2" s="53"/>
+      <c r="BI2" s="53"/>
+      <c r="BJ2" s="54"/>
+      <c r="BK2" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="BL2" s="54"/>
-      <c r="BM2" s="54"/>
-      <c r="BN2" s="54"/>
-      <c r="BO2" s="54"/>
-      <c r="BP2" s="54"/>
-      <c r="BQ2" s="55"/>
-      <c r="BR2" s="59" t="s">
+      <c r="BL2" s="53"/>
+      <c r="BM2" s="53"/>
+      <c r="BN2" s="53"/>
+      <c r="BO2" s="53"/>
+      <c r="BP2" s="53"/>
+      <c r="BQ2" s="54"/>
+      <c r="BR2" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="BS2" s="54"/>
-      <c r="BT2" s="54"/>
-      <c r="BU2" s="54"/>
-      <c r="BV2" s="54"/>
-      <c r="BW2" s="54"/>
-      <c r="BX2" s="55"/>
-      <c r="BY2" s="59" t="s">
+      <c r="BS2" s="53"/>
+      <c r="BT2" s="53"/>
+      <c r="BU2" s="53"/>
+      <c r="BV2" s="53"/>
+      <c r="BW2" s="53"/>
+      <c r="BX2" s="54"/>
+      <c r="BY2" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="BZ2" s="54"/>
-      <c r="CA2" s="54"/>
-      <c r="CB2" s="54"/>
-      <c r="CC2" s="54"/>
-      <c r="CD2" s="54"/>
-      <c r="CE2" s="55"/>
-      <c r="CF2" s="59" t="s">
+      <c r="BZ2" s="53"/>
+      <c r="CA2" s="53"/>
+      <c r="CB2" s="53"/>
+      <c r="CC2" s="53"/>
+      <c r="CD2" s="53"/>
+      <c r="CE2" s="54"/>
+      <c r="CF2" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="CG2" s="54"/>
-      <c r="CH2" s="54"/>
-      <c r="CI2" s="54"/>
-      <c r="CJ2" s="54"/>
-      <c r="CK2" s="54"/>
-      <c r="CL2" s="55"/>
-      <c r="CM2" s="59" t="s">
+      <c r="CG2" s="53"/>
+      <c r="CH2" s="53"/>
+      <c r="CI2" s="53"/>
+      <c r="CJ2" s="53"/>
+      <c r="CK2" s="53"/>
+      <c r="CL2" s="54"/>
+      <c r="CM2" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="CN2" s="54"/>
-      <c r="CO2" s="54"/>
-      <c r="CP2" s="54"/>
-      <c r="CQ2" s="54"/>
-      <c r="CR2" s="54"/>
-      <c r="CS2" s="55"/>
-      <c r="CT2" s="59" t="s">
+      <c r="CN2" s="53"/>
+      <c r="CO2" s="53"/>
+      <c r="CP2" s="53"/>
+      <c r="CQ2" s="53"/>
+      <c r="CR2" s="53"/>
+      <c r="CS2" s="54"/>
+      <c r="CT2" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="CU2" s="54"/>
-      <c r="CV2" s="54"/>
-      <c r="CW2" s="54"/>
-      <c r="CX2" s="54"/>
-      <c r="CY2" s="54"/>
-      <c r="CZ2" s="55"/>
+      <c r="CU2" s="53"/>
+      <c r="CV2" s="53"/>
+      <c r="CW2" s="53"/>
+      <c r="CX2" s="53"/>
+      <c r="CY2" s="53"/>
+      <c r="CZ2" s="54"/>
     </row>
     <row r="3" spans="1:104" x14ac:dyDescent="0.25">
-      <c r="G3" s="56">
+      <c r="G3" s="60">
         <f>G5</f>
         <v>42107</v>
       </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="60">
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="55">
         <f>N5</f>
         <v>42114</v>
       </c>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="58"/>
-      <c r="U3" s="60">
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="55">
         <f>U5</f>
         <v>42121</v>
       </c>
-      <c r="V3" s="57"/>
-      <c r="W3" s="57"/>
-      <c r="X3" s="57"/>
-      <c r="Y3" s="57"/>
-      <c r="Z3" s="57"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="60">
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="57"/>
+      <c r="AB3" s="55">
         <f>AB5</f>
         <v>42128</v>
       </c>
-      <c r="AC3" s="57"/>
-      <c r="AD3" s="57"/>
-      <c r="AE3" s="57"/>
-      <c r="AF3" s="57"/>
-      <c r="AG3" s="57"/>
-      <c r="AH3" s="58"/>
-      <c r="AI3" s="60">
+      <c r="AC3" s="56"/>
+      <c r="AD3" s="56"/>
+      <c r="AE3" s="56"/>
+      <c r="AF3" s="56"/>
+      <c r="AG3" s="56"/>
+      <c r="AH3" s="57"/>
+      <c r="AI3" s="55">
         <f>AI5</f>
         <v>42135</v>
       </c>
-      <c r="AJ3" s="57"/>
-      <c r="AK3" s="57"/>
-      <c r="AL3" s="57"/>
-      <c r="AM3" s="57"/>
-      <c r="AN3" s="57"/>
-      <c r="AO3" s="58"/>
-      <c r="AP3" s="60">
+      <c r="AJ3" s="56"/>
+      <c r="AK3" s="56"/>
+      <c r="AL3" s="56"/>
+      <c r="AM3" s="56"/>
+      <c r="AN3" s="56"/>
+      <c r="AO3" s="57"/>
+      <c r="AP3" s="55">
         <f>AP5</f>
         <v>42142</v>
       </c>
-      <c r="AQ3" s="57"/>
-      <c r="AR3" s="57"/>
-      <c r="AS3" s="57"/>
-      <c r="AT3" s="57"/>
-      <c r="AU3" s="57"/>
-      <c r="AV3" s="58"/>
-      <c r="AW3" s="60">
+      <c r="AQ3" s="56"/>
+      <c r="AR3" s="56"/>
+      <c r="AS3" s="56"/>
+      <c r="AT3" s="56"/>
+      <c r="AU3" s="56"/>
+      <c r="AV3" s="57"/>
+      <c r="AW3" s="55">
         <f t="shared" ref="AW3" si="0">AW5</f>
         <v>42149</v>
       </c>
-      <c r="AX3" s="57"/>
-      <c r="AY3" s="57"/>
-      <c r="AZ3" s="57"/>
-      <c r="BA3" s="57"/>
-      <c r="BB3" s="57"/>
-      <c r="BC3" s="58"/>
-      <c r="BD3" s="60">
+      <c r="AX3" s="56"/>
+      <c r="AY3" s="56"/>
+      <c r="AZ3" s="56"/>
+      <c r="BA3" s="56"/>
+      <c r="BB3" s="56"/>
+      <c r="BC3" s="57"/>
+      <c r="BD3" s="55">
         <f t="shared" ref="BD3" si="1">BD5</f>
         <v>42156</v>
       </c>
-      <c r="BE3" s="57"/>
-      <c r="BF3" s="57"/>
-      <c r="BG3" s="57"/>
-      <c r="BH3" s="57"/>
-      <c r="BI3" s="57"/>
-      <c r="BJ3" s="58"/>
-      <c r="BK3" s="60">
+      <c r="BE3" s="56"/>
+      <c r="BF3" s="56"/>
+      <c r="BG3" s="56"/>
+      <c r="BH3" s="56"/>
+      <c r="BI3" s="56"/>
+      <c r="BJ3" s="57"/>
+      <c r="BK3" s="55">
         <f t="shared" ref="BK3" si="2">BK5</f>
         <v>42163</v>
       </c>
-      <c r="BL3" s="57"/>
-      <c r="BM3" s="57"/>
-      <c r="BN3" s="57"/>
-      <c r="BO3" s="57"/>
-      <c r="BP3" s="57"/>
-      <c r="BQ3" s="58"/>
-      <c r="BR3" s="60">
+      <c r="BL3" s="56"/>
+      <c r="BM3" s="56"/>
+      <c r="BN3" s="56"/>
+      <c r="BO3" s="56"/>
+      <c r="BP3" s="56"/>
+      <c r="BQ3" s="57"/>
+      <c r="BR3" s="55">
         <f t="shared" ref="BR3" si="3">BR5</f>
         <v>42170</v>
       </c>
-      <c r="BS3" s="57"/>
-      <c r="BT3" s="57"/>
-      <c r="BU3" s="57"/>
-      <c r="BV3" s="57"/>
-      <c r="BW3" s="57"/>
-      <c r="BX3" s="58"/>
-      <c r="BY3" s="60">
+      <c r="BS3" s="56"/>
+      <c r="BT3" s="56"/>
+      <c r="BU3" s="56"/>
+      <c r="BV3" s="56"/>
+      <c r="BW3" s="56"/>
+      <c r="BX3" s="57"/>
+      <c r="BY3" s="55">
         <f t="shared" ref="BY3" si="4">BY5</f>
         <v>42177</v>
       </c>
-      <c r="BZ3" s="57"/>
-      <c r="CA3" s="57"/>
-      <c r="CB3" s="57"/>
-      <c r="CC3" s="57"/>
-      <c r="CD3" s="57"/>
-      <c r="CE3" s="58"/>
-      <c r="CF3" s="60">
+      <c r="BZ3" s="56"/>
+      <c r="CA3" s="56"/>
+      <c r="CB3" s="56"/>
+      <c r="CC3" s="56"/>
+      <c r="CD3" s="56"/>
+      <c r="CE3" s="57"/>
+      <c r="CF3" s="55">
         <f t="shared" ref="CF3" si="5">CF5</f>
         <v>42184</v>
       </c>
-      <c r="CG3" s="57"/>
-      <c r="CH3" s="57"/>
-      <c r="CI3" s="57"/>
-      <c r="CJ3" s="57"/>
-      <c r="CK3" s="57"/>
-      <c r="CL3" s="58"/>
-      <c r="CM3" s="60">
+      <c r="CG3" s="56"/>
+      <c r="CH3" s="56"/>
+      <c r="CI3" s="56"/>
+      <c r="CJ3" s="56"/>
+      <c r="CK3" s="56"/>
+      <c r="CL3" s="57"/>
+      <c r="CM3" s="55">
         <f t="shared" ref="CM3" si="6">CM5</f>
         <v>42191</v>
       </c>
-      <c r="CN3" s="57"/>
-      <c r="CO3" s="57"/>
-      <c r="CP3" s="57"/>
-      <c r="CQ3" s="57"/>
-      <c r="CR3" s="57"/>
-      <c r="CS3" s="58"/>
-      <c r="CT3" s="60">
+      <c r="CN3" s="56"/>
+      <c r="CO3" s="56"/>
+      <c r="CP3" s="56"/>
+      <c r="CQ3" s="56"/>
+      <c r="CR3" s="56"/>
+      <c r="CS3" s="57"/>
+      <c r="CT3" s="55">
         <f t="shared" ref="CT3" si="7">CT5</f>
         <v>42198</v>
       </c>
-      <c r="CU3" s="57"/>
-      <c r="CV3" s="57"/>
-      <c r="CW3" s="57"/>
-      <c r="CX3" s="57"/>
-      <c r="CY3" s="57"/>
-      <c r="CZ3" s="58"/>
+      <c r="CU3" s="56"/>
+      <c r="CV3" s="56"/>
+      <c r="CW3" s="56"/>
+      <c r="CX3" s="56"/>
+      <c r="CY3" s="56"/>
+      <c r="CZ3" s="57"/>
     </row>
     <row r="4" spans="1:104" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
@@ -22481,19 +22484,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="CT2:CZ2"/>
-    <mergeCell ref="CM3:CS3"/>
-    <mergeCell ref="CT3:CZ3"/>
-    <mergeCell ref="BY2:CE2"/>
-    <mergeCell ref="CF2:CL2"/>
-    <mergeCell ref="BY3:CE3"/>
-    <mergeCell ref="CF3:CL3"/>
-    <mergeCell ref="CM2:CS2"/>
-    <mergeCell ref="BD3:BJ3"/>
-    <mergeCell ref="BK2:BQ2"/>
-    <mergeCell ref="BR2:BX2"/>
-    <mergeCell ref="BK3:BQ3"/>
-    <mergeCell ref="BR3:BX3"/>
     <mergeCell ref="A1:CY1"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="G3:M3"/>
@@ -22510,6 +22500,19 @@
     <mergeCell ref="AI3:AO3"/>
     <mergeCell ref="AP3:AV3"/>
     <mergeCell ref="AW3:BC3"/>
+    <mergeCell ref="BD3:BJ3"/>
+    <mergeCell ref="BK2:BQ2"/>
+    <mergeCell ref="BR2:BX2"/>
+    <mergeCell ref="BK3:BQ3"/>
+    <mergeCell ref="BR3:BX3"/>
+    <mergeCell ref="CT2:CZ2"/>
+    <mergeCell ref="CM3:CS3"/>
+    <mergeCell ref="CT3:CZ3"/>
+    <mergeCell ref="BY2:CE2"/>
+    <mergeCell ref="CF2:CL2"/>
+    <mergeCell ref="BY3:CE3"/>
+    <mergeCell ref="CF3:CL3"/>
+    <mergeCell ref="CM2:CS2"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:CW300">
     <cfRule type="expression" dxfId="14" priority="77">
@@ -45845,8 +45848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45886,7 +45889,7 @@
       </c>
       <c r="H3">
         <f>SUM(Table1345[Time Spent (hours)])</f>
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -46110,6 +46113,12 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>224</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
       <c r="C24" t="s">
         <v>220</v>
       </c>

</xml_diff>